<commit_message>
added univ and publ data
</commit_message>
<xml_diff>
--- a/data/du/original_data/apc_du_2017_2018.xlsx
+++ b/data/du/original_data/apc_du_2017_2018.xlsx
@@ -20,8 +20,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Camilla Lindelöw</author>
+  </authors>
+  <commentList>
+    <comment ref="F11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Camilla Lindelöw:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+förlag tillagt på KB/CHL 180705</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="95">
   <si>
     <t>institution</t>
   </si>
@@ -155,9 +189,6 @@
     <t>http://www.mdpi.com/1996-1944/10/3/221</t>
   </si>
   <si>
-    <t>Finns ej - predatory journal</t>
-  </si>
-  <si>
     <t>Gavin Publishers</t>
   </si>
   <si>
@@ -215,9 +246,6 @@
     <t>10.1080/2331186X.2017.1349562</t>
   </si>
   <si>
-    <t>Finns ej</t>
-  </si>
-  <si>
     <t>T&amp;K Academic</t>
   </si>
   <si>
@@ -260,9 +288,6 @@
     <t>10.1080/09638288.2017.1406008</t>
   </si>
   <si>
-    <t>Ej publicerad ännu</t>
-  </si>
-  <si>
     <t>Hindawi</t>
   </si>
   <si>
@@ -314,14 +339,14 @@
     <t>ieee</t>
   </si>
   <si>
-    <t>förlag tillagt på KB/CHL 180705</t>
+    <t>10.1155/2018/8720643</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +373,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -687,11 +725,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -941,24 +979,22 @@
       <c r="C8" s="3">
         <v>3000</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" t="s">
         <v>45</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="I8" s="2"/>
       <c r="K8" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -972,7 +1008,7 @@
         <v>1600</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>12</v>
@@ -981,7 +1017,7 @@
         <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -989,7 +1025,7 @@
         <v>20</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1003,7 +1039,7 @@
         <v>2053</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>23</v>
@@ -1012,17 +1048,17 @@
         <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" t="s">
         <v>53</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1036,7 +1072,7 @@
         <v>1329</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>12</v>
@@ -1059,7 +1095,7 @@
         <v>1150</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>23</v>
@@ -1082,13 +1118,13 @@
         <v>1955</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1105,7 +1141,7 @@
         <v>2650</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>23</v>
@@ -1128,13 +1164,13 @@
         <v>2103</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1151,13 +1187,13 @@
         <v>2000</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1174,13 +1210,13 @@
         <v>2626</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1197,13 +1233,13 @@
         <v>1201</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -1219,25 +1255,23 @@
       <c r="C19" s="3">
         <v>260</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="D19" s="4"/>
       <c r="E19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1251,7 +1285,7 @@
         <v>3670</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>23</v>
@@ -1274,13 +1308,13 @@
         <v>1313</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1297,13 +1331,13 @@
         <v>1300</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1320,13 +1354,13 @@
         <v>2150</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1343,13 +1377,13 @@
         <v>2150</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1366,13 +1400,13 @@
         <v>205</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1389,13 +1423,13 @@
         <v>489</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1412,13 +1446,13 @@
         <v>1820</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1435,7 +1469,7 @@
         <v>1500</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>23</v>
@@ -1458,13 +1492,13 @@
         <v>2400</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -1481,13 +1515,13 @@
         <v>2150</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -1504,26 +1538,26 @@
         <v>867</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J31" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1537,13 +1571,13 @@
         <v>1650</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -1551,13 +1585,12 @@
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" s="6"/>
-      <c r="E35" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="E35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>